<commit_message>
automatic reading and normalising
To change which variables to include and how to normalise change values in kwb-variables.xlsx
</commit_message>
<xml_diff>
--- a/data/kwb-variables.xlsx
+++ b/data/kwb-variables.xlsx
@@ -8,27 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a7c7a2f2bd441bd3/Documents/Studie/Block 3/Spatial Statistics and Machine Learning/Covid_sewage_project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="234" documentId="11_F25DC773A252ABDACC104872695871CE5ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85604791-7470-47A7-9360-6404FCD3F76E}"/>
+  <xr:revisionPtr revIDLastSave="289" documentId="11_F25DC773A252ABDACC104872695871CE5ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4987BD1-1634-4628-BDD6-5FCCCF4A5787}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kwb-variables" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'kwb-variables'!$A$1:$C$118</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'kwb-variables'!$A$1:$F$118</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="249">
   <si>
     <t>Variabelenaam</t>
   </si>
@@ -772,6 +782,9 @@
   </si>
   <si>
     <t>Include</t>
+  </si>
+  <si>
+    <t>Need to normalise</t>
   </si>
 </sst>
 </file>
@@ -1095,11 +1108,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E118"/>
+  <dimension ref="A1:F118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,7 +1125,7 @@
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1126,10 +1139,13 @@
         <v>247</v>
       </c>
       <c r="E1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1142,11 +1158,14 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1159,11 +1178,14 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1176,11 +1198,14 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1193,11 +1218,14 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1208,13 +1236,16 @@
         <v>244</v>
       </c>
       <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1227,11 +1258,14 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1244,11 +1278,14 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1261,11 +1298,14 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1278,11 +1318,14 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1295,11 +1338,14 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1312,11 +1358,14 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1329,11 +1378,14 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1346,11 +1398,14 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1360,11 +1415,17 @@
       <c r="C15" t="s">
         <v>1</v>
       </c>
-      <c r="E15" t="s">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -1374,11 +1435,17 @@
       <c r="C16" t="s">
         <v>1</v>
       </c>
-      <c r="E16" t="s">
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1388,11 +1455,17 @@
       <c r="C17" t="s">
         <v>1</v>
       </c>
-      <c r="E17" t="s">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1405,11 +1478,14 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -1422,11 +1498,14 @@
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -1439,11 +1518,14 @@
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -1456,11 +1538,14 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -1473,11 +1558,14 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -1490,11 +1578,14 @@
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -1507,11 +1598,14 @@
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>61</v>
       </c>
@@ -1524,11 +1618,14 @@
       <c r="D25">
         <v>1</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -1538,8 +1635,11 @@
       <c r="C26" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -1552,11 +1652,14 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -1566,8 +1669,11 @@
       <c r="C28" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -1580,11 +1686,14 @@
       <c r="D29">
         <v>1</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -1597,11 +1706,14 @@
       <c r="D30">
         <v>1</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -1614,11 +1726,14 @@
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -1631,11 +1746,14 @@
       <c r="D32">
         <v>1</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -1648,11 +1766,14 @@
       <c r="D33">
         <v>1</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -1665,11 +1786,14 @@
       <c r="D34">
         <v>1</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -1683,7 +1807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -1693,8 +1817,11 @@
       <c r="C36" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>85</v>
       </c>
@@ -1704,11 +1831,17 @@
       <c r="C37" t="s">
         <v>2</v>
       </c>
-      <c r="E37" t="s">
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -1721,11 +1854,14 @@
       <c r="D38">
         <v>1</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>89</v>
       </c>
@@ -1738,11 +1874,14 @@
       <c r="D39">
         <v>1</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>91</v>
       </c>
@@ -1752,11 +1891,17 @@
       <c r="C40" t="s">
         <v>2</v>
       </c>
-      <c r="E40" t="s">
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>93</v>
       </c>
@@ -1766,11 +1911,17 @@
       <c r="C41" t="s">
         <v>2</v>
       </c>
-      <c r="E41" t="s">
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>95</v>
       </c>
@@ -1780,8 +1931,11 @@
       <c r="C42" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>97</v>
       </c>
@@ -1791,8 +1945,11 @@
       <c r="C43" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>99</v>
       </c>
@@ -1802,8 +1959,11 @@
       <c r="C44" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>101</v>
       </c>
@@ -1813,8 +1973,11 @@
       <c r="C45" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -1824,8 +1987,11 @@
       <c r="C46" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>105</v>
       </c>
@@ -1835,8 +2001,11 @@
       <c r="C47" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>107</v>
       </c>
@@ -1846,8 +2015,11 @@
       <c r="C48" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>109</v>
       </c>
@@ -1857,8 +2029,11 @@
       <c r="C49" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>111</v>
       </c>
@@ -1868,8 +2043,11 @@
       <c r="C50" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>113</v>
       </c>
@@ -1879,8 +2057,11 @@
       <c r="C51" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>115</v>
       </c>
@@ -1890,8 +2071,11 @@
       <c r="C52" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>117</v>
       </c>
@@ -1901,8 +2085,11 @@
       <c r="C53" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>119</v>
       </c>
@@ -1912,8 +2099,11 @@
       <c r="C54" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>121</v>
       </c>
@@ -1923,8 +2113,11 @@
       <c r="C55" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>123</v>
       </c>
@@ -1934,8 +2127,11 @@
       <c r="C56" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>125</v>
       </c>
@@ -1945,8 +2141,11 @@
       <c r="C57" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>127</v>
       </c>
@@ -1956,8 +2155,11 @@
       <c r="C58" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>128</v>
       </c>
@@ -1967,8 +2169,11 @@
       <c r="C59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>129</v>
       </c>
@@ -1978,8 +2183,11 @@
       <c r="C60" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>130</v>
       </c>
@@ -1989,8 +2197,11 @@
       <c r="C61" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -2000,8 +2211,11 @@
       <c r="C62" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>132</v>
       </c>
@@ -2011,8 +2225,11 @@
       <c r="C63" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>133</v>
       </c>
@@ -2022,8 +2239,11 @@
       <c r="C64" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>134</v>
       </c>
@@ -2033,8 +2253,11 @@
       <c r="C65" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>136</v>
       </c>
@@ -2047,11 +2270,14 @@
       <c r="D66">
         <v>1</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>138</v>
       </c>
@@ -2064,11 +2290,14 @@
       <c r="D67">
         <v>1</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>140</v>
       </c>
@@ -2081,11 +2310,14 @@
       <c r="D68">
         <v>1</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>142</v>
       </c>
@@ -2098,11 +2330,14 @@
       <c r="D69">
         <v>1</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>144</v>
       </c>
@@ -2115,11 +2350,14 @@
       <c r="D70">
         <v>1</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>146</v>
       </c>
@@ -2132,11 +2370,14 @@
       <c r="D71">
         <v>1</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>148</v>
       </c>
@@ -2149,11 +2390,14 @@
       <c r="D72">
         <v>1</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>150</v>
       </c>
@@ -2166,11 +2410,14 @@
       <c r="D73">
         <v>1</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>152</v>
       </c>
@@ -2183,11 +2430,14 @@
       <c r="D74">
         <v>1</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>154</v>
       </c>
@@ -2197,8 +2447,11 @@
       <c r="C75" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>156</v>
       </c>
@@ -2208,8 +2461,11 @@
       <c r="C76" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>158</v>
       </c>
@@ -2223,7 +2479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>160</v>
       </c>
@@ -2233,8 +2489,11 @@
       <c r="C78" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>162</v>
       </c>
@@ -2244,8 +2503,11 @@
       <c r="C79" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>164</v>
       </c>
@@ -2258,11 +2520,14 @@
       <c r="D80">
         <v>1</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>166</v>
       </c>
@@ -2275,11 +2540,14 @@
       <c r="D81">
         <v>1</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>168</v>
       </c>
@@ -2292,11 +2560,14 @@
       <c r="D82">
         <v>1</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>170</v>
       </c>
@@ -2309,11 +2580,14 @@
       <c r="D83">
         <v>1</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>172</v>
       </c>
@@ -2323,8 +2597,11 @@
       <c r="C84" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>174</v>
       </c>
@@ -2337,11 +2614,14 @@
       <c r="D85">
         <v>1</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85">
+        <v>1</v>
+      </c>
+      <c r="F85" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>176</v>
       </c>
@@ -2354,11 +2634,14 @@
       <c r="D86">
         <v>1</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>178</v>
       </c>
@@ -2371,11 +2654,14 @@
       <c r="D87">
         <v>1</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>180</v>
       </c>
@@ -2388,11 +2674,14 @@
       <c r="D88">
         <v>1</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>182</v>
       </c>
@@ -2402,8 +2691,11 @@
       <c r="C89" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>184</v>
       </c>
@@ -2416,11 +2708,14 @@
       <c r="D90">
         <v>1</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>186</v>
       </c>
@@ -2430,8 +2725,11 @@
       <c r="C91" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>188</v>
       </c>
@@ -2444,11 +2742,14 @@
       <c r="D92">
         <v>1</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>190</v>
       </c>
@@ -2458,8 +2759,11 @@
       <c r="C93" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>192</v>
       </c>
@@ -2469,8 +2773,11 @@
       <c r="C94" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>194</v>
       </c>
@@ -2480,8 +2787,11 @@
       <c r="C95" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>196</v>
       </c>
@@ -2491,8 +2801,11 @@
       <c r="C96" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>198</v>
       </c>
@@ -2502,8 +2815,11 @@
       <c r="C97" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>200</v>
       </c>
@@ -2513,8 +2829,11 @@
       <c r="C98" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>202</v>
       </c>
@@ -2524,8 +2843,11 @@
       <c r="C99" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>204</v>
       </c>
@@ -2535,8 +2857,11 @@
       <c r="C100" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>206</v>
       </c>
@@ -2546,8 +2871,11 @@
       <c r="C101" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>208</v>
       </c>
@@ -2557,8 +2885,11 @@
       <c r="C102" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>210</v>
       </c>
@@ -2568,8 +2899,11 @@
       <c r="C103" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>212</v>
       </c>
@@ -2579,8 +2913,11 @@
       <c r="C104" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>214</v>
       </c>
@@ -2590,8 +2927,11 @@
       <c r="C105" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>216</v>
       </c>
@@ -2601,8 +2941,11 @@
       <c r="C106" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>218</v>
       </c>
@@ -2615,11 +2958,14 @@
       <c r="D107">
         <v>1</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>220</v>
       </c>
@@ -2629,8 +2975,11 @@
       <c r="C108" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>222</v>
       </c>
@@ -2640,8 +2989,11 @@
       <c r="C109" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>224</v>
       </c>
@@ -2651,8 +3003,11 @@
       <c r="C110" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>226</v>
       </c>
@@ -2665,11 +3020,14 @@
       <c r="D111">
         <v>1</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="F111" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>228</v>
       </c>
@@ -2679,8 +3037,11 @@
       <c r="C112" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>230</v>
       </c>
@@ -2690,8 +3051,11 @@
       <c r="C113" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>232</v>
       </c>
@@ -2701,8 +3065,11 @@
       <c r="C114" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>234</v>
       </c>
@@ -2712,8 +3079,11 @@
       <c r="C115" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>236</v>
       </c>
@@ -2723,8 +3093,11 @@
       <c r="C116" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>238</v>
       </c>
@@ -2734,8 +3107,11 @@
       <c r="C117" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>240</v>
       </c>
@@ -2745,9 +3121,12 @@
       <c r="C118" t="s">
         <v>14</v>
       </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C118" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F118" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
outcome  plot, corr, lm, morran's I
</commit_message>
<xml_diff>
--- a/data/kwb-variables.xlsx
+++ b/data/kwb-variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a7c7a2f2bd441bd3/Documents/Studie/Block 3/Spatial Statistics and Machine Learning/Covid_sewage_project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="289" documentId="11_F25DC773A252ABDACC104872695871CE5ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4987BD1-1634-4628-BDD6-5FCCCF4A5787}"/>
+  <xr:revisionPtr revIDLastSave="303" documentId="11_F25DC773A252ABDACC104872695871CE5ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FAB10A3-E9D8-49C7-BE88-52F621D3379F}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1108,11 +1108,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A66:A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,7 +1226,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1405,7 +1406,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1425,7 +1426,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -1445,7 +1446,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1625,7 +1626,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -1659,7 +1660,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -1807,7 +1808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -1821,7 +1822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>85</v>
       </c>
@@ -1881,7 +1882,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>91</v>
       </c>
@@ -1901,7 +1902,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>93</v>
       </c>
@@ -1921,7 +1922,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>95</v>
       </c>
@@ -1935,7 +1936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>97</v>
       </c>
@@ -1949,7 +1950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>99</v>
       </c>
@@ -1963,7 +1964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>101</v>
       </c>
@@ -1977,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -1991,7 +1992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>105</v>
       </c>
@@ -2005,7 +2006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>107</v>
       </c>
@@ -2019,7 +2020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>109</v>
       </c>
@@ -2033,7 +2034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>111</v>
       </c>
@@ -2047,7 +2048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>113</v>
       </c>
@@ -2061,7 +2062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>115</v>
       </c>
@@ -2075,7 +2076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>117</v>
       </c>
@@ -2089,7 +2090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>119</v>
       </c>
@@ -2103,7 +2104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>121</v>
       </c>
@@ -2117,7 +2118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>123</v>
       </c>
@@ -2131,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>125</v>
       </c>
@@ -2145,7 +2146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>127</v>
       </c>
@@ -2159,7 +2160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>128</v>
       </c>
@@ -2173,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>129</v>
       </c>
@@ -2187,7 +2188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>130</v>
       </c>
@@ -2201,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -2215,7 +2216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>132</v>
       </c>
@@ -2229,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>133</v>
       </c>
@@ -2243,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>134</v>
       </c>
@@ -2317,7 +2318,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>142</v>
       </c>
@@ -2328,7 +2329,7 @@
         <v>5</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -2337,7 +2338,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>144</v>
       </c>
@@ -2348,7 +2349,7 @@
         <v>5</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -2357,7 +2358,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>146</v>
       </c>
@@ -2368,7 +2369,7 @@
         <v>5</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -2377,7 +2378,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>148</v>
       </c>
@@ -2388,7 +2389,7 @@
         <v>6</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -2397,7 +2398,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>150</v>
       </c>
@@ -2408,7 +2409,7 @@
         <v>6</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -2417,7 +2418,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>152</v>
       </c>
@@ -2428,7 +2429,7 @@
         <v>6</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -2437,7 +2438,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>154</v>
       </c>
@@ -2451,7 +2452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>156</v>
       </c>
@@ -2465,7 +2466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>158</v>
       </c>
@@ -2476,10 +2477,10 @@
         <v>6</v>
       </c>
       <c r="D77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>160</v>
       </c>
@@ -2493,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>162</v>
       </c>
@@ -2507,7 +2508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>164</v>
       </c>
@@ -2518,7 +2519,7 @@
         <v>6</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -2527,7 +2528,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>166</v>
       </c>
@@ -2538,7 +2539,7 @@
         <v>6</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -2547,7 +2548,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>168</v>
       </c>
@@ -2558,7 +2559,7 @@
         <v>6</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -2567,7 +2568,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>170</v>
       </c>
@@ -2578,7 +2579,7 @@
         <v>6</v>
       </c>
       <c r="D83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E83">
         <v>1</v>
@@ -2587,7 +2588,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>172</v>
       </c>
@@ -2681,7 +2682,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>182</v>
       </c>
@@ -2715,7 +2716,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>186</v>
       </c>
@@ -2749,7 +2750,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>190</v>
       </c>
@@ -2763,7 +2764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>192</v>
       </c>
@@ -2777,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>194</v>
       </c>
@@ -2791,7 +2792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>196</v>
       </c>
@@ -2805,7 +2806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>198</v>
       </c>
@@ -2819,7 +2820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>200</v>
       </c>
@@ -2833,7 +2834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>202</v>
       </c>
@@ -2847,7 +2848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>204</v>
       </c>
@@ -2861,7 +2862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>206</v>
       </c>
@@ -2875,7 +2876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>208</v>
       </c>
@@ -2889,7 +2890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>210</v>
       </c>
@@ -2903,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>212</v>
       </c>
@@ -2917,7 +2918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>214</v>
       </c>
@@ -2931,7 +2932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>216</v>
       </c>
@@ -2965,7 +2966,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>220</v>
       </c>
@@ -2979,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>222</v>
       </c>
@@ -2993,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>224</v>
       </c>
@@ -3027,7 +3028,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>228</v>
       </c>
@@ -3041,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>230</v>
       </c>
@@ -3055,7 +3056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>232</v>
       </c>
@@ -3069,7 +3070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>234</v>
       </c>
@@ -3083,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>236</v>
       </c>
@@ -3097,7 +3098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>238</v>
       </c>
@@ -3111,7 +3112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>240</v>
       </c>
@@ -3126,7 +3127,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F118" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F118" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>